<commit_message>
removed pre-push hook as flawed logic
</commit_message>
<xml_diff>
--- a/leetcode_solutions.xlsx
+++ b/leetcode_solutions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Question No.</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>Difficulty</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Given an array of integers nums and an integer target, return indices of the two numbers such that they add up to target.</t>
+  </si>
+  <si>
+    <t>Hash Map</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
 </sst>
 </file>
@@ -408,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -432,6 +450,26 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove solution from excel file
</commit_message>
<xml_diff>
--- a/leetcode_solutions.xlsx
+++ b/leetcode_solutions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Question No.</t>
   </si>
@@ -20,9 +20,6 @@
   </si>
   <si>
     <t>Problem Statement</t>
-  </si>
-  <si>
-    <t>Solution</t>
   </si>
   <si>
     <t>Technique</t>
@@ -426,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,29 +444,26 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>